<commit_message>
Added all files for the Macao
</commit_message>
<xml_diff>
--- a/BOM/Severus/Severus_BOM_Control_and_Price_Tracking.xlsx
+++ b/BOM/Severus/Severus_BOM_Control_and_Price_Tracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudy\OneDrive\PhD\Publications\Conference 1 - IEEE EMBC 2026\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rudy\OneDrive\PhD\VS Code\Prosthetic-Hands\Prosthetic-Hands\BOM\Severus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47500BB1-4D68-4B8D-ADC0-73861163FF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7185C27E-1E77-4647-A052-1C00E0CC0319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{043B56EA-62B9-4C47-8B29-ED9E1364A12F}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Part</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>RS</t>
+  </si>
+  <si>
+    <t>BOM Control and Price Tracking - Severus</t>
   </si>
 </sst>
 </file>
@@ -321,16 +324,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -339,12 +333,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -701,16 +704,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2"/>
@@ -1073,11 +1076,11 @@
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1">
         <f>SUM($F$4:$F30)</f>
@@ -1085,11 +1088,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="2"/>
       <c r="E32" s="1" cm="1">
         <f t="array" ref="E32">SUM($B$4:$B30*$G$4:$G30)</f>
@@ -1122,16 +1125,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1163,7 +1166,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,841 +1185,841 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="A1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2"/>
       <c r="E2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="8">
         <v>18.989999999999998</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>0.35</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <f>B4*E4</f>
         <v>6.6464999999999987</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="9">
         <v>1</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="9">
         <v>0.7</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="9">
         <f>H4-I4</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>8.9499999999999993</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>0.03</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <f t="shared" ref="F5:F30" si="0">B5*E5</f>
         <v>0.26849999999999996</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="9">
         <v>1</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="9">
         <v>1</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="9">
         <v>0.05</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="9">
         <f t="shared" ref="J5:J30" si="1">H5-I5</f>
         <v>0.95</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="8">
         <f>1.19/100</f>
         <v>1.1899999999999999E-2</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>15</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>0.17849999999999999</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="9">
         <v>100</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>100</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="9">
         <v>6</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="9">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="8">
         <f>11.99/1600</f>
         <v>7.4937500000000004E-3</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>46</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>0.34471250000000003</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="9">
         <v>1600</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="9">
         <v>1600</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="9">
         <v>60</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="9">
         <f t="shared" si="1"/>
         <v>1540</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="8">
         <f>6/20</f>
         <v>0.3</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="9">
         <v>15</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="9">
         <v>20</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <v>20</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="9">
         <v>19</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="8">
         <f>10.02/100</f>
         <v>0.1002</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12">
+      <c r="D9" s="7"/>
+      <c r="E9" s="9">
         <v>30</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>3.0059999999999998</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="9">
         <v>100</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="9">
         <v>100</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="9">
         <v>36</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="9">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="8">
         <v>11.5</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12">
+      <c r="D10" s="7"/>
+      <c r="E10" s="9">
         <v>5</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>57.5</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="9">
         <v>5</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="9">
         <v>5</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="9">
         <v>5</v>
       </c>
-      <c r="J10" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="13" t="s">
+      <c r="J10" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="8">
         <v>11.5</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12">
+      <c r="D11" s="7"/>
+      <c r="E11" s="9">
         <v>1</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="9">
         <v>2</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="9">
         <v>2</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="9">
         <v>1</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="8">
         <f>7.99/100</f>
         <v>7.9899999999999999E-2</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="12">
+      <c r="D12" s="7"/>
+      <c r="E12" s="9">
         <v>6</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>0.47939999999999999</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <v>100</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="9">
         <v>100</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="9">
         <v>8</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="9">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="8">
         <v>0.01</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="12">
+      <c r="D13" s="7"/>
+      <c r="E13" s="9">
         <v>6</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="10"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="8">
         <v>0.01</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="12">
+      <c r="D14" s="7"/>
+      <c r="E14" s="9">
         <v>6</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="10"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="8">
         <v>0.01</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="12">
+      <c r="D15" s="7"/>
+      <c r="E15" s="9">
         <v>6</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="10"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="8">
         <v>15.9</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="12">
+      <c r="D16" s="7"/>
+      <c r="E16" s="9">
         <v>1</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <f t="shared" si="0"/>
         <v>15.9</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="9">
         <v>1</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="9">
         <v>1</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="9">
         <v>1</v>
       </c>
-      <c r="J16" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="13" t="s">
+      <c r="J16" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="8">
         <v>5.8</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="12">
+      <c r="D17" s="7"/>
+      <c r="E17" s="9">
         <v>3</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="9">
         <v>3</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="9">
         <v>3</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="9">
         <v>3</v>
       </c>
-      <c r="J17" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="13" t="s">
+      <c r="J17" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="8">
         <f>7.57/100</f>
         <v>7.5700000000000003E-2</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>5</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <f t="shared" si="0"/>
         <v>0.3785</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="9">
         <v>100</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="9">
         <v>100</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="9">
         <v>12</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="9">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="K18" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="10"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="10"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="10"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="10"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="10"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="10"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="10"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="10"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="10"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="10"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="10"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="10"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16">
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12">
         <f>SUM($F$4:$F30)</f>
         <v>118.28211250000001</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="17"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16" cm="1">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12" cm="1">
         <f t="array" ref="E32">SUM($B$4:$B30*$G$4:$G30)</f>
         <v>186.5</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="17"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>